<commit_message>
Mudanças na inserção de dados e switch para nubucípios
</commit_message>
<xml_diff>
--- a/OcorrenciaMensal(Criminal)-Itanhaém_2025.xlsx
+++ b/OcorrenciaMensal(Criminal)-Itanhaém_2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_peres_sptech_school/Documents/sptech/Projeto PI - 2 Semestre/vigilante-backend/Base de dados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/guilherme_peres_sptech_school/Documents/sptech/Projeto PI - 2 Semestre/vigilante-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_BF389575B05F6E8A399050AD04C7FF4EDC8D2AFB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{248CFBB0-B9CD-4F25-94AC-FF99D94D8753}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_BF389575B05F6E8A399050AD04C7FF4EDC8D2AFB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{260EA7B7-E1BB-414C-BDF1-9B7B03D818F4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,10 +259,10 @@
     <t>Município</t>
   </si>
   <si>
-    <t>Itanhém</t>
-  </si>
-  <si>
     <t>Ano</t>
+  </si>
+  <si>
+    <t>Itanhaém</t>
   </si>
 </sst>
 </file>
@@ -324,10 +324,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -650,7 +646,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,7 +698,7 @@
         <v>78</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -749,7 +745,7 @@
         <v>18</v>
       </c>
       <c r="O2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="P2" s="2">
         <v>2025</v>

</xml_diff>